<commit_message>
Changed complete algorithm structure and fixed all errors, working version
</commit_message>
<xml_diff>
--- a/apps/workflow-py/workflow/outputs/top15_perfecte_woningen_tabel_final.xlsx
+++ b/apps/workflow-py/workflow/outputs/top15_perfecte_woningen_tabel_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,11 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Tuin</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Score</t>
         </is>
       </c>
@@ -476,25 +481,26 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Elandsgracht 41, 1016TV, Amsterdam</t>
+          <t>Nieuwe Leliestraat 97, 1015SL, Amsterdam</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1475000</v>
+        <v>925000</v>
       </c>
       <c r="D2" t="n">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.96</v>
+        <v>2</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>0.8392333333333335</v>
       </c>
     </row>
     <row r="3">
@@ -503,25 +509,26 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Lijnbaansgracht 1183V, 1016VV, Amsterdam</t>
+          <t>Nieuwe Leliestraat 8H, 1015SP, Amsterdam</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>725000</v>
+        <v>895000</v>
       </c>
       <c r="D3" t="n">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.9386363636363636</v>
+        <v>2</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>0.8192333333333334</v>
       </c>
     </row>
     <row r="4">
@@ -530,25 +537,26 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Akoleienstraat 81, 1016LN, Amsterdam</t>
+          <t>Oude Looiersstraat 382, 1016VJ, Amsterdam</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>725000</v>
+        <v>795000</v>
       </c>
       <c r="D4" t="n">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.9261363636363636</v>
+        <v>2</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>0.8102627450980394</v>
       </c>
     </row>
     <row r="5">
@@ -557,25 +565,26 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Elandsgracht 103A, 1016TS, Amsterdam</t>
+          <t>Tweede Bloemdwarsstraat 34A, 1016LM, Amsterdam</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>950000</v>
+        <v>750000</v>
       </c>
       <c r="D5" t="n">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F5" t="n">
         <v>3</v>
       </c>
-      <c r="G5" t="n">
-        <v>0.9097727272727272</v>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>0.7978000000000002</v>
       </c>
     </row>
     <row r="6">
@@ -584,25 +593,26 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Eerste Leliedwarsstraat 5, 1015SZ, Amsterdam</t>
+          <t>Akoleienstraat 81, 1016LN, Amsterdam</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>850000</v>
+        <v>725000</v>
       </c>
       <c r="D6" t="n">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F6" t="n">
         <v>3</v>
       </c>
-      <c r="G6" t="n">
-        <v>0.9086363636363636</v>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>0.7966000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -611,25 +621,26 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lijnbaansgracht 2043, 1016XA, Amsterdam</t>
+          <t>Laurierstraat 26H, 1016PM, Amsterdam</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>750000</v>
+        <v>949000</v>
       </c>
       <c r="D7" t="n">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.906818181818182</v>
+        <v>2</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>0.7940627450980393</v>
       </c>
     </row>
     <row r="8">
@@ -638,25 +649,26 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Nieuwe Leliestraat 168H, 1015HE, Amsterdam</t>
+          <t>Laurierstraat 11B, 1016PG, Amsterdam</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>745000</v>
+        <v>1100000</v>
       </c>
       <c r="D8" t="n">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.8747727272727273</v>
+        <v>2</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>0.7940627450980393</v>
       </c>
     </row>
     <row r="9">
@@ -665,25 +677,26 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Lauriergracht 1142, 1016RR, Amsterdam</t>
+          <t>Oude Looiersstraat 372, 1016VG, Amsterdam</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1250000</v>
+        <v>660000</v>
       </c>
       <c r="D9" t="n">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.8724999999999999</v>
+        <v>2</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>0.7927627450980393</v>
       </c>
     </row>
     <row r="10">
@@ -692,25 +705,26 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Tweede Bloemdwarsstraat 34A, 1016LM, Amsterdam</t>
+          <t>Elandsgracht 103A, 1016TS, Amsterdam</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>750000</v>
+        <v>950000</v>
       </c>
       <c r="D10" t="n">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F10" t="n">
         <v>3</v>
       </c>
-      <c r="G10" t="n">
-        <v>0.8711363636363637</v>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="n">
+        <v>0.7876294117647061</v>
       </c>
     </row>
     <row r="11">
@@ -719,25 +733,26 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lauriergracht 1263, 1016RS, Amsterdam</t>
+          <t>Tweede Bloemdwarsstraat 92, 1016LL, Amsterdam</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>615000</v>
+        <v>799000</v>
       </c>
       <c r="D11" t="n">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.8586363636363638</v>
+        <v>2</v>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>0.7786333333333335</v>
       </c>
     </row>
     <row r="12">
@@ -746,25 +761,26 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rozengracht 225D, 1016NA, Amsterdam</t>
+          <t>Nieuwe Leliestraat 168H, 1015HE, Amsterdam</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>795000</v>
+        <v>745000</v>
       </c>
       <c r="D12" t="n">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.856969696969697</v>
+        <v>3</v>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="n">
+        <v>0.7759000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -773,25 +789,26 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hazenstraat 12, 1016SP, Amsterdam</t>
+          <t>Tweede Leliedwarsstraat 16, 1015TC, Amsterdam</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1000000</v>
+        <v>775000</v>
       </c>
       <c r="D13" t="n">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F13" t="n">
         <v>2</v>
       </c>
-      <c r="G13" t="n">
-        <v>0.8501515151515152</v>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="n">
+        <v>0.7717333333333335</v>
       </c>
     </row>
     <row r="14">
@@ -800,25 +817,26 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bloemstraat 83, 1016KX, Amsterdam</t>
+          <t>Bloemstraat 1211, 1016KZ, Amsterdam</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1750000</v>
+        <v>950000</v>
       </c>
       <c r="D14" t="n">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>3</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0.8222727272727274</v>
+        <v>2</v>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="n">
+        <v>0.7693333333333334</v>
       </c>
     </row>
     <row r="15">
@@ -827,25 +845,26 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bloemstraat 1211, 1016KZ, Amsterdam</t>
+          <t>Egelantiersgracht 101A, 1015RG, Amsterdam</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>950000</v>
+        <v>850000</v>
       </c>
       <c r="D15" t="n">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.8212878787878789</v>
+        <v>3</v>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="n">
+        <v>0.7666000000000002</v>
       </c>
     </row>
     <row r="16">
@@ -854,25 +873,26 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Elandsstraat 58, 1016SG, Amsterdam</t>
+          <t>Lauriergracht 1142, 1016RR, Amsterdam</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>900000</v>
+        <v>1250000</v>
       </c>
       <c r="D16" t="n">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0.8131060606060607</v>
+        <v>3</v>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="n">
+        <v>0.766429411764706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjustments, more accurate price calculation, working program
</commit_message>
<xml_diff>
--- a/apps/workflow-py/workflow/outputs/top15_perfecte_woningen_tabel_final.xlsx
+++ b/apps/workflow-py/workflow/outputs/top15_perfecte_woningen_tabel_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,10 +466,30 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Badkamers</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Bouwjaar</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>Tuin</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Onderhoud Binnen</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Onderhoud Buiten</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Score</t>
         </is>
@@ -481,26 +501,44 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nieuwe Leliestraat 97, 1015SL, Amsterdam</t>
+          <t xml:space="preserve"> Gerard Doustraat 168 3, 1073 VZ Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>925000</v>
+        <v>690000</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
       <c r="H2" t="n">
-        <v>0.8392333333333335</v>
+        <v>1876</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>0.7345454545454545</v>
       </c>
     </row>
     <row r="3">
@@ -509,26 +547,44 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nieuwe Leliestraat 8H, 1015SP, Amsterdam</t>
+          <t xml:space="preserve"> Gerard Doustraat 2 3, 1072 VP Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>895000</v>
+        <v>800000</v>
       </c>
       <c r="D3" t="n">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>B</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
       <c r="H3" t="n">
-        <v>0.8192333333333334</v>
+        <v>1886</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>0.7272727272727272</v>
       </c>
     </row>
     <row r="4">
@@ -537,26 +593,44 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Oude Looiersstraat 382, 1016VJ, Amsterdam</t>
+          <t xml:space="preserve"> Quellijnstraat 56 3, 1072 XT Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>795000</v>
+        <v>649000</v>
       </c>
       <c r="D4" t="n">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
         <v>2</v>
       </c>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>0.8102627450980394</v>
+        <v>1906</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Uitstekend</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>0.6920833333333334</v>
       </c>
     </row>
     <row r="5">
@@ -565,26 +639,44 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tweede Bloemdwarsstraat 34A, 1016LM, Amsterdam</t>
+          <t xml:space="preserve"> Gerard Doustraat 3 A3, 1072 VH Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>750000</v>
+        <v>640000</v>
       </c>
       <c r="D5" t="n">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
       <c r="H5" t="n">
-        <v>0.7978000000000002</v>
+        <v>1880</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>0.6912121212121213</v>
       </c>
     </row>
     <row r="6">
@@ -593,26 +685,44 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Akoleienstraat 81, 1016LN, Amsterdam</t>
+          <t xml:space="preserve"> Gerard Doustraat 234 2, 1073 XC Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>725000</v>
+        <v>475000</v>
       </c>
       <c r="D6" t="n">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
       <c r="H6" t="n">
-        <v>0.7966000000000001</v>
+        <v>1892</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>0.6878787878787879</v>
       </c>
     </row>
     <row r="7">
@@ -621,26 +731,44 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Laurierstraat 26H, 1016PM, Amsterdam</t>
+          <t xml:space="preserve"> Eerste Sweelinckstraat 5 3, 1073 CK Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>949000</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
       <c r="H7" t="n">
-        <v>0.7940627450980393</v>
+        <v>1886</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>0.6833333333333333</v>
       </c>
     </row>
     <row r="8">
@@ -649,26 +777,44 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Laurierstraat 11B, 1016PG, Amsterdam</t>
+          <t xml:space="preserve"> Quellijnstraat 19 A, 1072 XM Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1100000</v>
+        <v>725000</v>
       </c>
       <c r="D8" t="n">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
       <c r="H8" t="n">
-        <v>0.7940627450980393</v>
+        <v>1879</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>0.6599621212121213</v>
       </c>
     </row>
     <row r="9">
@@ -677,26 +823,44 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Oude Looiersstraat 372, 1016VG, Amsterdam</t>
+          <t xml:space="preserve"> Gerard Doustraat 192 2, 1073 XA Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>660000</v>
+        <v>450000</v>
       </c>
       <c r="D9" t="n">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>D</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
       <c r="H9" t="n">
-        <v>0.7927627450980393</v>
+        <v>1906</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>0.6584848484848485</v>
       </c>
     </row>
     <row r="10">
@@ -705,26 +869,44 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Elandsgracht 103A, 1016TS, Amsterdam</t>
+          <t xml:space="preserve"> Quellijnstraat 17 3, 1072 XM Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>950000</v>
+        <v>675000</v>
       </c>
       <c r="D10" t="n">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
-      </c>
-      <c r="G10" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
       <c r="H10" t="n">
-        <v>0.7876294117647061</v>
+        <v>1879</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>0.6566287878787879</v>
       </c>
     </row>
     <row r="11">
@@ -733,26 +915,44 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Tweede Bloemdwarsstraat 92, 1016LL, Amsterdam</t>
+          <t xml:space="preserve"> Quellijnstraat 41 B, 1072 XP Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>799000</v>
+        <v>785000</v>
       </c>
       <c r="D11" t="n">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
       <c r="H11" t="n">
-        <v>0.7786333333333335</v>
+        <v>1906</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>0.6554166666666668</v>
       </c>
     </row>
     <row r="12">
@@ -761,14 +961,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Nieuwe Leliestraat 168H, 1015HE, Amsterdam</t>
+          <t xml:space="preserve"> Gerard Doustraat 147 E, 1073 VV Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>745000</v>
+        <v>800000</v>
       </c>
       <c r="D12" t="n">
-        <v>126</v>
+        <v>87</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -776,11 +976,29 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>3</v>
-      </c>
-      <c r="G12" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
       <c r="H12" t="n">
-        <v>0.7759000000000001</v>
+        <v>2010</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>0.6549999999999999</v>
       </c>
     </row>
     <row r="13">
@@ -789,26 +1007,44 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Tweede Leliedwarsstraat 16, 1015TC, Amsterdam</t>
+          <t xml:space="preserve"> Quellijnstraat 37 B, 1072 XP Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>775000</v>
+        <v>725000</v>
       </c>
       <c r="D13" t="n">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>B</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
       <c r="H13" t="n">
-        <v>0.7717333333333335</v>
+        <v>1879</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>0.652689393939394</v>
       </c>
     </row>
     <row r="14">
@@ -817,26 +1053,44 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bloemstraat 1211, 1016KZ, Amsterdam</t>
+          <t xml:space="preserve"> Gerard Doustraat 82 3, 1072 VW Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>950000</v>
+        <v>565000</v>
       </c>
       <c r="D14" t="n">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>G</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
       <c r="H14" t="n">
-        <v>0.7693333333333334</v>
+        <v>1876</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>0.646969696969697</v>
       </c>
     </row>
     <row r="15">
@@ -845,26 +1099,44 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Egelantiersgracht 101A, 1015RG, Amsterdam</t>
+          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 32 3, 1072 TV Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>850000</v>
+        <v>750000</v>
       </c>
       <c r="D15" t="n">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
       <c r="H15" t="n">
-        <v>0.7666000000000002</v>
+        <v>1906</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>0.640625</v>
       </c>
     </row>
     <row r="16">
@@ -873,26 +1145,44 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Lauriergracht 1142, 1016RR, Amsterdam</t>
+          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 42 1, 1072 TV Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1250000</v>
+        <v>675000</v>
       </c>
       <c r="D16" t="n">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>3</v>
-      </c>
-      <c r="G16" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
       <c r="H16" t="n">
-        <v>0.766429411764706</v>
+        <v>1906</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Goed</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>0.6372916666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest changes on Main for correct version
</commit_message>
<xml_diff>
--- a/apps/workflow-py/workflow/outputs/top15_perfecte_woningen_tabel_final.xlsx
+++ b/apps/workflow-py/workflow/outputs/top15_perfecte_woningen_tabel_final.xlsx
@@ -501,35 +501,35 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gerard Doustraat 168 3, 1073 VZ Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Quellijnstraat 56 3, 1072 XT Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>690000</v>
+        <v>649000</v>
       </c>
       <c r="D2" t="n">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>1876</v>
+        <v>1906</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Goed</t>
+          <t>Uitstekend</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0.7345454545454545</v>
+        <v>0.6920833333333334</v>
       </c>
     </row>
     <row r="3">
@@ -547,25 +547,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gerard Doustraat 2 3, 1072 VP Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Eerste Sweelinckstraat 5 3, 1073 CK Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>800000</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
         <v>1886</v>
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>0.7272727272727272</v>
+        <v>0.6833333333333333</v>
       </c>
     </row>
     <row r="4">
@@ -593,35 +593,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 56 3, 1072 XT Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Quellijnstraat 19 A, 1072 XM Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>649000</v>
+        <v>725000</v>
       </c>
       <c r="D4" t="n">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>1906</v>
+        <v>1879</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Uitstekend</t>
+          <t>Goed</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0.6920833333333334</v>
+        <v>0.6599621212121213</v>
       </c>
     </row>
     <row r="5">
@@ -639,14 +639,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gerard Doustraat 3 A3, 1072 VH Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Quellijnstraat 17 3, 1072 XM Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>640000</v>
+        <v>675000</v>
       </c>
       <c r="D5" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -657,10 +657,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>0.6912121212121213</v>
+        <v>0.6566287878787879</v>
       </c>
     </row>
     <row r="6">
@@ -685,18 +685,18 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gerard Doustraat 234 2, 1073 XC Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Quellijnstraat 41 B, 1072 XP Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>475000</v>
+        <v>785000</v>
       </c>
       <c r="D6" t="n">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>1892</v>
+        <v>1906</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>0.6878787878787879</v>
+        <v>0.6554166666666668</v>
       </c>
     </row>
     <row r="7">
@@ -731,28 +731,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Sweelinckstraat 5 3, 1073 CK Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Quellijnstraat 37 B, 1072 XP Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>725000</v>
       </c>
       <c r="D7" t="n">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>1886</v>
+        <v>1879</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>0.6833333333333333</v>
+        <v>0.652689393939394</v>
       </c>
     </row>
     <row r="8">
@@ -777,18 +777,18 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 19 A, 1072 XM Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 32 3, 1072 TV Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>725000</v>
+        <v>750000</v>
       </c>
       <c r="D8" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>1879</v>
+        <v>1906</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0.6599621212121213</v>
+        <v>0.640625</v>
       </c>
     </row>
     <row r="9">
@@ -823,18 +823,18 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gerard Doustraat 192 2, 1073 XA Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 42 1, 1072 TV Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>450000</v>
+        <v>675000</v>
       </c>
       <c r="D9" t="n">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>0.6584848484848485</v>
+        <v>0.6372916666666668</v>
       </c>
     </row>
     <row r="10">
@@ -869,18 +869,18 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 17 3, 1072 XM Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 42 5, 1072 TV Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>675000</v>
+        <v>725000</v>
       </c>
       <c r="D10" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -890,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>1879</v>
+        <v>1906</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -906,7 +906,7 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>0.6566287878787879</v>
+        <v>0.6372916666666668</v>
       </c>
     </row>
     <row r="11">
@@ -915,14 +915,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 41 B, 1072 XP Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 48 1, 1072 TW Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>785000</v>
+        <v>695000</v>
       </c>
       <c r="D11" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>0.6554166666666668</v>
+        <v>0.6372916666666668</v>
       </c>
     </row>
     <row r="12">
@@ -961,18 +961,18 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gerard Doustraat 147 E, 1073 VV Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 44 1, 1072 TW Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>800000</v>
+        <v>675000</v>
       </c>
       <c r="D12" t="n">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -982,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>2010</v>
+        <v>1906</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>0.6549999999999999</v>
+        <v>0.6372916666666668</v>
       </c>
     </row>
     <row r="13">
@@ -1007,18 +1007,18 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 37 B, 1072 XP Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 36 C, 1072 TV Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>725000</v>
+        <v>699000</v>
       </c>
       <c r="D13" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>1879</v>
+        <v>1896</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
@@ -1044,7 +1044,7 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>0.652689393939394</v>
+        <v>0.6339583333333334</v>
       </c>
     </row>
     <row r="14">
@@ -1053,18 +1053,18 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Gerard Doustraat 82 3, 1072 VW Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Quellijnstraat 82 H, 1072 XX Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>565000</v>
+        <v>425000</v>
       </c>
       <c r="D14" t="n">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1074,7 +1074,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>1876</v>
+        <v>1879</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="L14" t="n">
-        <v>0.646969696969697</v>
+        <v>0.6332954545454546</v>
       </c>
     </row>
     <row r="15">
@@ -1099,18 +1099,18 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 32 3, 1072 TV Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Quellijnstraat 104 1, 1072 XZ Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>750000</v>
+        <v>675000</v>
       </c>
       <c r="D15" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1120,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>1906</v>
+        <v>1879</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
@@ -1136,7 +1136,7 @@
         </is>
       </c>
       <c r="L15" t="n">
-        <v>0.640625</v>
+        <v>0.6232954545454547</v>
       </c>
     </row>
     <row r="16">
@@ -1145,18 +1145,18 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 42 1, 1072 TV Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 36 F, 1072 TV Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>675000</v>
+        <v>875000</v>
       </c>
       <c r="D16" t="n">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1166,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>1906</v>
+        <v>1896</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>0.6372916666666668</v>
+        <v>0.6212310606060606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest adjustments, working program
</commit_message>
<xml_diff>
--- a/apps/workflow-py/workflow/outputs/top15_perfecte_woningen_tabel_final.xlsx
+++ b/apps/workflow-py/workflow/outputs/top15_perfecte_woningen_tabel_final.xlsx
@@ -501,18 +501,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 56 3, 1072 XT Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Churchill-laan 290 2, 1078 GB Amsterdam Verkocht onder voorbehoud </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>649000</v>
+        <v>870000</v>
       </c>
       <c r="D2" t="n">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -522,14 +522,14 @@
         <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>1906</v>
+        <v>1926</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Uitstekend</t>
+          <t>Goed</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>0.6920833333333334</v>
+        <v>0.7941636363636363</v>
       </c>
     </row>
     <row r="3">
@@ -547,28 +547,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Sweelinckstraat 5 3, 1073 CK Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Churchill-laan 157 2, 1078 DV Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>675000</v>
       </c>
       <c r="D3" t="n">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>1886</v>
+        <v>1928</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>0.6833333333333333</v>
+        <v>0.7797636363636363</v>
       </c>
     </row>
     <row r="4">
@@ -593,14 +593,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 19 A, 1072 XM Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Churchill-laan 153 4, 1078 DT Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>725000</v>
+        <v>795000</v>
       </c>
       <c r="D4" t="n">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -614,7 +614,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>1879</v>
+        <v>1928</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>0.6599621212121213</v>
+        <v>0.7617636363636363</v>
       </c>
     </row>
     <row r="5">
@@ -639,14 +639,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 17 3, 1072 XM Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Scheldestraat 29 1, 1078 GE Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>675000</v>
+        <v>850000</v>
       </c>
       <c r="D5" t="n">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -660,7 +660,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>1879</v>
+        <v>1928</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>0.6566287878787879</v>
+        <v>0.7547922077922078</v>
       </c>
     </row>
     <row r="6">
@@ -685,18 +685,18 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 41 B, 1072 XP Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Churchill-laan 119 4, 1078 DN Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>785000</v>
+        <v>675000</v>
       </c>
       <c r="D6" t="n">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>1906</v>
+        <v>1928</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>0.6554166666666668</v>
+        <v>0.7545636363636363</v>
       </c>
     </row>
     <row r="7">
@@ -731,18 +731,18 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 37 B, 1072 XP Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Churchill-laan 282 3, 1078 GB Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>725000</v>
+        <v>795000</v>
       </c>
       <c r="D7" t="n">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>1879</v>
+        <v>1929</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>0.652689393939394</v>
+        <v>0.7537454545454545</v>
       </c>
     </row>
     <row r="8">
@@ -777,18 +777,18 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 32 3, 1072 TV Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Scheldestraat 29 4, 1078 GE Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>750000</v>
+        <v>700000</v>
       </c>
       <c r="D8" t="n">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>1906</v>
+        <v>1928</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>0.640625</v>
+        <v>0.7486103896103896</v>
       </c>
     </row>
     <row r="9">
@@ -823,18 +823,18 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 42 1, 1072 TV Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Rooseveltlaan 168 2, 1078 NT Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>675000</v>
+        <v>875000</v>
       </c>
       <c r="D9" t="n">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -844,7 +844,7 @@
         <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>1906</v>
+        <v>1934</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>0.6372916666666668</v>
+        <v>0.7477636363636363</v>
       </c>
     </row>
     <row r="10">
@@ -869,18 +869,18 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 42 5, 1072 TV Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Rooseveltlaan 224 III, 1078 NX Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>725000</v>
+        <v>800000</v>
       </c>
       <c r="D10" t="n">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -890,23 +890,23 @@
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>1906</v>
+        <v>1934</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Goed</t>
+          <t>Uitstekend</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Goed</t>
+          <t>Uitstekend</t>
         </is>
       </c>
       <c r="L10" t="n">
-        <v>0.6372916666666668</v>
+        <v>0.7441636363636364</v>
       </c>
     </row>
     <row r="11">
@@ -915,14 +915,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 48 1, 1072 TW Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Rooseveltlaan 230 3, 1078 NX Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>695000</v>
+        <v>895000</v>
       </c>
       <c r="D11" t="n">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -936,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>1906</v>
+        <v>1934</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>0.6372916666666668</v>
+        <v>0.7428000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -961,44 +961,44 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 44 1, 1072 TW Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Churchill-laan 248 1, 1078 EZ Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>675000</v>
+        <v>750000</v>
       </c>
       <c r="D12" t="n">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>1906</v>
+        <v>1928</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Goed</t>
+          <t>Matig</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Goed</t>
+          <t>Matig</t>
         </is>
       </c>
       <c r="L12" t="n">
-        <v>0.6372916666666668</v>
+        <v>0.742</v>
       </c>
     </row>
     <row r="13">
@@ -1007,18 +1007,18 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 36 C, 1072 TV Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Churchill-laan 161 H, 1078 DV Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>699000</v>
+        <v>995000</v>
       </c>
       <c r="D13" t="n">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1028,10 +1028,10 @@
         <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>1896</v>
+        <v>1928</v>
       </c>
       <c r="I13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1044,7 +1044,7 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>0.6339583333333334</v>
+        <v>0.7385454545454547</v>
       </c>
     </row>
     <row r="14">
@@ -1053,14 +1053,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 82 H, 1072 XX Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Churchill-laan 59 B, 1078 DH Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>425000</v>
+        <v>715000</v>
       </c>
       <c r="D14" t="n">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1071,26 +1071,26 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>1879</v>
+        <v>1927</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Goed</t>
+          <t>Uitstekend</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Goed</t>
+          <t>Uitstekend</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>0.6332954545454546</v>
+        <v>0.7295636363636364</v>
       </c>
     </row>
     <row r="15">
@@ -1099,14 +1099,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Quellijnstraat 104 1, 1072 XZ Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Rooseveltlaan 122 1, 1078 NP Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>675000</v>
+        <v>899000</v>
       </c>
       <c r="D15" t="n">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1117,26 +1117,26 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" t="n">
-        <v>1879</v>
+        <v>1930</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Goed</t>
+          <t>Uitstekend</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Goed</t>
+          <t>Uitstekend</t>
         </is>
       </c>
       <c r="L15" t="n">
-        <v>0.6232954545454547</v>
+        <v>0.7227636363636363</v>
       </c>
     </row>
     <row r="16">
@@ -1145,18 +1145,18 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Eerste Jan van der Heijdenstraat 36 F, 1072 TV Amsterdam Verkocht Width</t>
+          <t xml:space="preserve"> Amstelkade 168 2, 1078 AZ Amsterdam Verkocht Width</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>875000</v>
+        <v>850000</v>
       </c>
       <c r="D16" t="n">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>D</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1166,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>1896</v>
+        <v>1936</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>0.6212310606060606</v>
+        <v>0.7180597402597403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>